<commit_message>
Updates to Provenance and PDex Device
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pdex-provenance.xlsx
+++ b/output/StructureDefinition-pdex-provenance.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$35</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="270">
   <si>
     <t>Path</t>
   </si>
@@ -322,33 +322,54 @@
     <t>Provenance.extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>sourceFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/davinci-pdex/ImplementationGuide/davinci-pdex/StructureDefinition/ProvenanceConversionFrom}
+</t>
+  </si>
+  <si>
+    <t>Source format resource was converted from</t>
+  </si>
+  <si>
+    <t>Optional Extension Element - found in all resources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>Provenance.modifierExtension</t>
+  </si>
+  <si>
     <t>extensions
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Provenance.modifierExtension</t>
-  </si>
-  <si>
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
@@ -356,6 +377,9 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
     <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
@@ -612,6 +636,9 @@
     <t>Provenance.agent.extension</t>
   </si>
   <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
     <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
@@ -650,7 +677,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/provenance-agent-type</t>
+    <t>http://hl7.org/fhir/ValueSet/ValueSet-ProvenancePayerAgent</t>
   </si>
   <si>
     <t>Event.performer.function</t>
@@ -975,7 +1002,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN34"/>
+  <dimension ref="A1:AN35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1008,7 +1035,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="36.81640625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="56.35546875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="59.60546875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
@@ -1950,7 +1977,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -1969,17 +1996,15 @@
         <v>44</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="L9" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>102</v>
-      </c>
+      <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
         <v>44</v>
@@ -2016,16 +2041,14 @@
         <v>44</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB9" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="AE9" t="s" s="2">
         <v>103</v>
@@ -2046,7 +2069,7 @@
         <v>44</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>44</v>
@@ -2060,43 +2083,41 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>44</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M10" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N10" t="s" s="2">
         <v>108</v>
       </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>44</v>
       </c>
@@ -2144,7 +2165,7 @@
         <v>44</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>42</v>
@@ -2153,7 +2174,7 @@
         <v>43</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="AI10" t="s" s="2">
         <v>104</v>
@@ -2180,11 +2201,11 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>43</v>
@@ -2193,13 +2214,13 @@
         <v>44</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="K11" t="s" s="2">
         <v>112</v>
@@ -2210,7 +2231,9 @@
       <c r="M11" t="s" s="2">
         <v>114</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="O11" t="s" s="2">
         <v>44</v>
       </c>
@@ -2258,10 +2281,10 @@
         <v>44</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>43</v>
@@ -2270,27 +2293,27 @@
         <v>44</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>116</v>
+        <v>44</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>118</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2298,10 +2321,10 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>44</v>
@@ -2310,19 +2333,19 @@
         <v>44</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J12" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="L12" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="K12" t="s" s="2">
+      <c r="M12" t="s" s="2">
         <v>121</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>123</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -2360,23 +2383,25 @@
         <v>44</v>
       </c>
       <c r="AA12" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="AB12" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC12" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD12" t="s" s="2">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH12" t="s" s="2">
         <v>44</v>
@@ -2385,28 +2410,26 @@
         <v>65</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>44</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
         <v>44</v>
       </c>
@@ -2427,16 +2450,16 @@
         <v>44</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -2474,19 +2497,17 @@
         <v>44</v>
       </c>
       <c r="AA13" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB13" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="AB13" s="2"/>
       <c r="AC13" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD13" t="s" s="2">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>42</v>
@@ -2501,16 +2522,16 @@
         <v>65</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>44</v>
@@ -2518,15 +2539,17 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>137</v>
+      </c>
       <c r="C14" t="s" s="2">
         <v>44</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>53</v>
@@ -2538,19 +2561,19 @@
         <v>44</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2600,10 +2623,10 @@
         <v>44</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>53</v>
@@ -2615,24 +2638,24 @@
         <v>65</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>44</v>
+        <v>133</v>
       </c>
       <c r="AK14" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AM14" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="AL14" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="AM14" t="s" s="2">
-        <v>138</v>
-      </c>
       <c r="AN14" t="s" s="2">
-        <v>139</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2640,10 +2663,10 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>44</v>
@@ -2652,19 +2675,19 @@
         <v>44</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="K15" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="L15" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>142</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>143</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -2714,13 +2737,13 @@
         <v>44</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>44</v>
@@ -2732,21 +2755,21 @@
         <v>44</v>
       </c>
       <c r="AK15" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AL15" t="s" s="2">
         <v>144</v>
       </c>
-      <c r="AL15" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="AM15" t="s" s="2">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2757,7 +2780,7 @@
         <v>42</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>44</v>
@@ -2769,7 +2792,7 @@
         <v>44</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>148</v>
@@ -2777,7 +2800,9 @@
       <c r="L16" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="M16" s="2"/>
+      <c r="M16" t="s" s="2">
+        <v>150</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
         <v>44</v>
@@ -2826,13 +2851,13 @@
         <v>44</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>44</v>
@@ -2841,24 +2866,24 @@
         <v>65</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>150</v>
+        <v>44</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>151</v>
       </c>
       <c r="AL16" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM16" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN16" t="s" s="2">
         <v>152</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>154</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2869,7 +2894,7 @@
         <v>42</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>44</v>
@@ -2881,13 +2906,13 @@
         <v>44</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>156</v>
-      </c>
-      <c r="K17" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2914,13 +2939,13 @@
         <v>44</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>160</v>
+        <v>44</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>161</v>
+        <v>44</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>44</v>
@@ -2938,13 +2963,13 @@
         <v>44</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>44</v>
@@ -2953,24 +2978,24 @@
         <v>65</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2981,7 +3006,7 @@
         <v>42</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>44</v>
@@ -2993,13 +3018,13 @@
         <v>44</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3026,13 +3051,13 @@
         <v>44</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>44</v>
@@ -3050,13 +3075,13 @@
         <v>44</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>44</v>
@@ -3065,19 +3090,19 @@
         <v>65</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AL18" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="AM18" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AN18" t="s" s="2">
         <v>173</v>
-      </c>
-      <c r="AL18" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="AN18" t="s" s="2">
-        <v>44</v>
       </c>
     </row>
     <row r="19" hidden="true">
@@ -3090,11 +3115,11 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="F19" t="s" s="2">
-        <v>43</v>
-      </c>
       <c r="G19" t="s" s="2">
         <v>44</v>
       </c>
@@ -3105,20 +3130,16 @@
         <v>44</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="L19" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>179</v>
-      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>44</v>
       </c>
@@ -3142,13 +3163,13 @@
         <v>44</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>44</v>
+        <v>177</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>44</v>
@@ -3169,10 +3190,10 @@
         <v>174</v>
       </c>
       <c r="AF19" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG19" t="s" s="2">
         <v>53</v>
-      </c>
-      <c r="AG19" t="s" s="2">
-        <v>43</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>44</v>
@@ -3181,24 +3202,24 @@
         <v>65</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="AK19" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="AK19" t="s" s="2">
-        <v>181</v>
-      </c>
       <c r="AL19" t="s" s="2">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>184</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3206,10 +3227,10 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>44</v>
@@ -3221,16 +3242,20 @@
         <v>44</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>55</v>
+        <v>182</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="M20" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="N20" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="L20" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>44</v>
       </c>
@@ -3278,50 +3303,50 @@
         <v>44</v>
       </c>
       <c r="AE20" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="AF20" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG20" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH20" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI20" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ20" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="AK20" t="s" s="2">
         <v>188</v>
       </c>
-      <c r="AF20" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG20" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH20" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI20" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ20" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AL20" t="s" s="2">
         <v>189</v>
       </c>
-      <c r="AL20" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="AM20" t="s" s="2">
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>44</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s" s="2">
         <v>44</v>
@@ -3333,17 +3358,15 @@
         <v>44</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>44</v>
@@ -3392,25 +3415,25 @@
         <v>44</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>44</v>
@@ -3424,11 +3447,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -3441,26 +3464,24 @@
         <v>44</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>44</v>
       </c>
@@ -3508,7 +3529,7 @@
         <v>44</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>42</v>
@@ -3526,7 +3547,7 @@
         <v>44</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>44</v>
@@ -3540,41 +3561,43 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="N23" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="O23" t="s" s="2">
         <v>44</v>
       </c>
@@ -3598,11 +3621,13 @@
         <v>44</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="X23" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="X23" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="Y23" t="s" s="2">
-        <v>203</v>
+        <v>44</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>44</v>
@@ -3620,39 +3645,39 @@
         <v>44</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>204</v>
+        <v>44</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>205</v>
+        <v>96</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>206</v>
+        <v>44</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>207</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3672,19 +3697,19 @@
         <v>44</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="M24" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>211</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3710,11 +3735,11 @@
         <v>44</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" t="s" s="2">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>44</v>
@@ -3732,13 +3757,13 @@
         <v>44</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>44</v>
@@ -3747,13 +3772,13 @@
         <v>65</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>44</v>
+        <v>212</v>
       </c>
       <c r="AK24" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="AL24" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="AL24" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>44</v>
@@ -3784,19 +3809,19 @@
         <v>44</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="K25" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="L25" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3822,13 +3847,11 @@
         <v>44</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X25" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="X25" s="2"/>
       <c r="Y25" t="s" s="2">
-        <v>44</v>
+        <v>221</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>44</v>
@@ -3849,10 +3872,10 @@
         <v>216</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>44</v>
@@ -3861,7 +3884,7 @@
         <v>65</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>221</v>
+        <v>44</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>222</v>
@@ -3870,10 +3893,10 @@
         <v>44</v>
       </c>
       <c r="AM25" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN25" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>44</v>
       </c>
     </row>
     <row r="26" hidden="true">
@@ -3886,7 +3909,7 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>53</v>
@@ -3898,19 +3921,19 @@
         <v>44</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -3963,7 +3986,7 @@
         <v>224</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>53</v>
@@ -3975,16 +3998,16 @@
         <v>65</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>44</v>
@@ -3992,7 +4015,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4003,7 +4026,7 @@
         <v>42</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>44</v>
@@ -4015,15 +4038,17 @@
         <v>44</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M27" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>235</v>
+      </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>44</v>
@@ -4072,13 +4097,13 @@
         <v>44</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>44</v>
@@ -4090,21 +4115,21 @@
         <v>44</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>233</v>
+        <v>44</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>234</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4115,7 +4140,7 @@
         <v>42</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>44</v>
@@ -4127,13 +4152,13 @@
         <v>44</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>55</v>
+        <v>182</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>186</v>
+        <v>238</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>187</v>
+        <v>239</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4184,50 +4209,50 @@
         <v>44</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>188</v>
+        <v>237</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>189</v>
+        <v>240</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>44</v>
+        <v>241</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>44</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>44</v>
@@ -4239,17 +4264,15 @@
         <v>44</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>44</v>
@@ -4298,25 +4321,25 @@
         <v>44</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>44</v>
@@ -4330,11 +4353,11 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
@@ -4347,26 +4370,24 @@
         <v>44</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>44</v>
       </c>
@@ -4414,7 +4435,7 @@
         <v>44</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>42</v>
@@ -4432,7 +4453,7 @@
         <v>44</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>44</v>
@@ -4446,39 +4467,43 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+        <v>204</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="N31" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="O31" t="s" s="2">
         <v>44</v>
       </c>
@@ -4502,13 +4527,13 @@
         <v>44</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>202</v>
+        <v>44</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>241</v>
+        <v>44</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>242</v>
+        <v>44</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>44</v>
@@ -4526,34 +4551,34 @@
         <v>44</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>243</v>
+        <v>96</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>244</v>
+        <v>44</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>245</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" hidden="true">
@@ -4581,7 +4606,7 @@
         <v>54</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>247</v>
@@ -4589,9 +4614,7 @@
       <c r="L32" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="M32" t="s" s="2">
-        <v>249</v>
-      </c>
+      <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>44</v>
@@ -4616,13 +4639,13 @@
         <v>44</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>44</v>
+        <v>249</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>44</v>
+        <v>250</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>44</v>
@@ -4658,21 +4681,21 @@
         <v>44</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>118</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4680,10 +4703,10 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>44</v>
@@ -4692,19 +4715,19 @@
         <v>44</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
@@ -4754,13 +4777,13 @@
         <v>44</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>44</v>
@@ -4772,21 +4795,21 @@
         <v>44</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>44</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4809,15 +4832,17 @@
         <v>44</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>258</v>
+        <v>44</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M34" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>263</v>
+      </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>44</v>
@@ -4866,7 +4891,7 @@
         <v>44</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>42</v>
@@ -4884,7 +4909,7 @@
         <v>44</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>44</v>
@@ -4893,11 +4918,123 @@
         <v>44</v>
       </c>
       <c r="AN34" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" hidden="true">
+      <c r="A35" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J35" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE35" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AL35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN35" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN34">
+  <autoFilter ref="A1:AN35">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -4907,7 +5044,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI33">
+  <conditionalFormatting sqref="A2:AI34">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Temporary Change ot base device and provenance off US Core profiles
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pdex-provenance.xlsx
+++ b/output/StructureDefinition-pdex-provenance.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$55</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="298">
   <si>
     <t>Path</t>
   </si>
@@ -141,7 +141,7 @@
   </si>
   <si>
     <t>History
-EventActivity</t>
+EventActivityBasic Provenance</t>
   </si>
   <si>
     <t>0</t>
@@ -153,10 +153,10 @@
     <t/>
   </si>
   <si>
-    <t>Who, What, When for a set of resources</t>
-  </si>
-  <si>
-    <t>Provenance of a resource is a record that describes entities and processes involved in producing and delivering or otherwise influencing that resource. Provenance provides a critical foundation for assessing authenticity, enabling trust, and allowing reproducibility. Provenance assertions are a form of contextual metadata and can themselves become important records with their own provenance. Provenance statement indicates clinical significance in terms of confidence in authenticity, reliability, and trustworthiness, integrity, and stage in lifecycle (e.g. Document Completion - has the artifact been legally authenticated), all of which may impact security, privacy, and trust policies.</t>
+    <t>US Core Provenance</t>
+  </si>
+  <si>
+    <t>The US Core Provenance Profile is based upon the Argonaut Data Query requirements.</t>
   </si>
   <si>
     <t>Some parties may be duplicated between the target resource and its provenance.  For instance, the prescriber is usually (but not always) the author of the prescription resource. This resource is defined with close consideration for W3C Provenance.</t>
@@ -470,7 +470,7 @@
 </t>
   </si>
   <si>
-    <t>Target Reference(s) (usually version specific)</t>
+    <t>The Resource this Provenance record supports</t>
   </si>
   <si>
     <t>The Reference(s) that were generated or updated by  the activity described in this resource. A provenance can point to more than one target if multiple resources were created/updated by the same activity.</t>
@@ -666,6 +666,10 @@
     <t>An agent can be a person, an organization, software, device, or other entities that may be ascribed responsibility.</t>
   </si>
   <si>
+    <t xml:space="preserve">pattern:type}
+</t>
+  </si>
+  <si>
     <t>Event.performer</t>
   </si>
   <si>
@@ -792,20 +796,62 @@
     <t>Provenance.agent.onBehalfOf</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization)
+</t>
+  </si>
+  <si>
+    <t>Who the agent is representing</t>
+  </si>
+  <si>
+    <t>The individual, device, or organization for whom the change was made.</t>
+  </si>
+  <si>
+    <t>onBehalfOfIdentity should be used when the agent is not a Resource type.</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+provenance-1:onBehalfOf SHALL be present when Provenance.agent.who is a Practitioner or Device {($this.agent.who.resolve().is Practitioner or Device) implies exists()}</t>
+  </si>
+  <si>
+    <t>Person, Practitioner, Organization, Device :* .role [classCode = RoleClassMutualRelationship; role.code and * .scopes[Role](classCode=IDENT) and *.plays [Role.Code]</t>
+  </si>
+  <si>
+    <t>ProvenanceAuthor</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://terminology.hl7.org/CodeSystem/provenance-participant-type"/&gt;
+    &lt;code value="author"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
+    <t>The type of participation that a provenance agent played with respect to the activity.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/provenance-agent-type</t>
+  </si>
+  <si>
+    <t>Who participated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reference(Practitioner|PractitionerRole|RelatedPerson|Patient|Device|Organization)
 </t>
   </si>
   <si>
-    <t>Who the agent is representing</t>
-  </si>
-  <si>
-    <t>The individual, device, or organization for whom the change was made.</t>
-  </si>
-  <si>
-    <t>onBehalfOfIdentity should be used when the agent is not a Resource type.</t>
-  </si>
-  <si>
-    <t>Person, Practitioner, Organization, Device :* .role [classCode = RoleClassMutualRelationship; role.code and * .scopes[Role](classCode=IDENT) and *.plays [Role.Code]</t>
+    <t>ProvenanceTransmitter</t>
+  </si>
+  <si>
+    <t>The entity that provided the copy to your system.</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://hl7.org/fhir/us/core/CodeSystem/us-core-provenance-participant-type"/&gt;
+    &lt;code value="transmitter"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>Provenance.entity</t>
@@ -1054,7 +1100,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN39"/>
+  <dimension ref="A1:AN55"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1064,7 +1110,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="35.328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.5" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="23.05078125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
@@ -1086,7 +1132,7 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="65.578125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="81.1875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="78.5703125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
@@ -2923,7 +2969,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>142</v>
       </c>
@@ -2939,7 +2985,7 @@
         <v>43</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>44</v>
@@ -3151,7 +3197,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
         <v>160</v>
       </c>
@@ -3167,7 +3213,7 @@
         <v>53</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>44</v>
@@ -3731,7 +3777,7 @@
         <v>43</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>44</v>
@@ -3789,16 +3835,14 @@
         <v>44</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB24" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="AB24" s="2"/>
       <c r="AC24" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="AE24" t="s" s="2">
         <v>202</v>
@@ -3816,24 +3860,24 @@
         <v>65</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3945,7 +3989,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3971,10 +4015,10 @@
         <v>98</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M26" t="s" s="2">
         <v>139</v>
@@ -4059,11 +4103,11 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -4085,10 +4129,10 @@
         <v>98</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M27" t="s" s="2">
         <v>139</v>
@@ -4143,7 +4187,7 @@
         <v>44</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>42</v>
@@ -4173,9 +4217,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4189,7 +4233,7 @@
         <v>53</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>44</v>
@@ -4201,13 +4245,13 @@
         <v>125</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4237,7 +4281,7 @@
       </c>
       <c r="X28" s="2"/>
       <c r="Y28" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>44</v>
@@ -4255,7 +4299,7 @@
         <v>44</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>42</v>
@@ -4270,24 +4314,24 @@
         <v>65</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4313,13 +4357,13 @@
         <v>125</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4345,13 +4389,13 @@
         <v>44</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>44</v>
@@ -4369,7 +4413,7 @@
         <v>44</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
@@ -4387,7 +4431,7 @@
         <v>44</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>44</v>
@@ -4396,12 +4440,12 @@
         <v>44</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4415,7 +4459,7 @@
         <v>53</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>44</v>
@@ -4424,16 +4468,16 @@
         <v>54</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4483,7 +4527,7 @@
         <v>44</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>53</v>
@@ -4498,24 +4542,24 @@
         <v>65</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="31" hidden="true">
+    <row r="31">
       <c r="A31" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4529,7 +4573,7 @@
         <v>53</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>44</v>
@@ -4538,16 +4582,16 @@
         <v>44</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4597,7 +4641,7 @@
         <v>44</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>42</v>
@@ -4609,13 +4653,13 @@
         <v>44</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>65</v>
+        <v>254</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>44</v>
@@ -4627,11 +4671,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>202</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>256</v>
+      </c>
       <c r="C32" t="s" s="2">
         <v>44</v>
       </c>
@@ -4643,7 +4689,7 @@
         <v>43</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>44</v>
@@ -4655,13 +4701,17 @@
         <v>203</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+        <v>205</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>207</v>
+      </c>
       <c r="O32" t="s" s="2">
         <v>44</v>
       </c>
@@ -4709,10 +4759,10 @@
         <v>44</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>43</v>
@@ -4724,24 +4774,24 @@
         <v>65</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>44</v>
+        <v>209</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>44</v>
+        <v>212</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>259</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>260</v>
+        <v>214</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4853,7 +4903,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>261</v>
+        <v>215</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4879,10 +4929,10 @@
         <v>98</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>139</v>
@@ -4967,11 +5017,11 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>262</v>
+        <v>218</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -4993,10 +5043,10 @@
         <v>98</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M35" t="s" s="2">
         <v>139</v>
@@ -5051,7 +5101,7 @@
         <v>44</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
@@ -5081,9 +5131,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5097,7 +5147,7 @@
         <v>53</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>44</v>
@@ -5106,15 +5156,17 @@
         <v>54</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>264</v>
+        <v>224</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="M36" s="2"/>
+        <v>225</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>226</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>44</v>
@@ -5124,7 +5176,7 @@
         <v>44</v>
       </c>
       <c r="R36" t="s" s="2">
-        <v>44</v>
+        <v>257</v>
       </c>
       <c r="S36" t="s" s="2">
         <v>44</v>
@@ -5139,13 +5191,13 @@
         <v>44</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>44</v>
@@ -5163,10 +5215,10 @@
         <v>44</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>53</v>
@@ -5178,24 +5230,24 @@
         <v>65</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>44</v>
+        <v>228</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>268</v>
+        <v>229</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>270</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5203,10 +5255,10 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>44</v>
@@ -5215,19 +5267,19 @@
         <v>44</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5253,13 +5305,13 @@
         <v>44</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>44</v>
+        <v>236</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>44</v>
+        <v>237</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>44</v>
+        <v>238</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>44</v>
@@ -5277,13 +5329,13 @@
         <v>44</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>44</v>
@@ -5295,21 +5347,21 @@
         <v>44</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>276</v>
+        <v>44</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>150</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5317,10 +5369,10 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>44</v>
@@ -5329,19 +5381,19 @@
         <v>44</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>44</v>
+        <v>242</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -5391,13 +5443,13 @@
         <v>44</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>44</v>
@@ -5406,16 +5458,16 @@
         <v>65</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>44</v>
+        <v>246</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>44</v>
+        <v>248</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>44</v>
@@ -5423,7 +5475,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5434,7 +5486,7 @@
         <v>42</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>44</v>
@@ -5446,15 +5498,17 @@
         <v>44</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="M39" s="2"/>
+        <v>252</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>253</v>
+      </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>44</v>
@@ -5503,13 +5557,13 @@
         <v>44</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>44</v>
@@ -5521,20 +5575,1842 @@
         <v>44</v>
       </c>
       <c r="AK39" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AL39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN39" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="C40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F40" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G40" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="H40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J40" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="O40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P40" s="2"/>
+      <c r="Q40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="AL40" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AM40" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AN40" t="s" s="2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" hidden="true">
+      <c r="A41" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F41" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J41" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P41" s="2"/>
+      <c r="Q41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN41" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J42" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="N42" s="2"/>
+      <c r="O42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P42" s="2"/>
+      <c r="Q42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE42" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="AL42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN42" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" hidden="true">
+      <c r="A43" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H43" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="I43" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J43" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P43" s="2"/>
+      <c r="Q43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN43" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F44" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G44" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="H44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I44" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J44" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="N44" s="2"/>
+      <c r="O44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P44" s="2"/>
+      <c r="Q44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R44" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="S44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W44" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="X44" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AL44" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="AM44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN44" t="s" s="2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" hidden="true">
+      <c r="A45" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F45" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="N45" s="2"/>
+      <c r="O45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P45" s="2"/>
+      <c r="Q45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE45" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AL45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN45" t="s" s="2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" hidden="true">
+      <c r="A46" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F46" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J46" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="N46" s="2"/>
+      <c r="O46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P46" s="2"/>
+      <c r="Q46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AN46" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" hidden="true">
+      <c r="A47" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F47" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="N47" s="2"/>
+      <c r="O47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P47" s="2"/>
+      <c r="Q47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" hidden="true">
+      <c r="A48" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F48" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P48" s="2"/>
+      <c r="Q48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="49" hidden="true">
+      <c r="A49" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F49" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J49" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P49" s="2"/>
+      <c r="Q49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" hidden="true">
+      <c r="A50" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F50" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="N50" s="2"/>
+      <c r="O50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P50" s="2"/>
+      <c r="Q50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN50" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" hidden="true">
+      <c r="A51" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F51" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H51" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J51" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE51" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="N53" s="2"/>
+      <c r="O53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK53" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="AL39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN39" t="s" s="2">
+      <c r="AL53" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="N54" s="2"/>
+      <c r="O54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN55" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN39">
+  <autoFilter ref="A1:AN55">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5544,7 +7420,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI38">
+  <conditionalFormatting sqref="A2:AI54">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update to 0.1.18 Simplified Server Capability Statement due to Publisher Issue (Timeout with sushi)
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pdex-provenance.xlsx
+++ b/output/StructureDefinition-pdex-provenance.xlsx
@@ -349,11 +349,11 @@
     <t>sourceFormat</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/ProvenanceConversionFrom}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/ProvenanceSourceFrom}
 </t>
   </si>
   <si>
-    <t>Source format resource was converted from</t>
+    <t>Source format target resource was created from</t>
   </si>
   <si>
     <t>Optional Extension Element - found in all resources.</t>
@@ -399,7 +399,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/ProvenanceConversionFrom</t>
+    <t>http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/ProvenanceSourceFrom</t>
   </si>
   <si>
     <t>Extension.url</t>

</xml_diff>

<commit_message>
0.1.29 Fix spelling error in SourceFormat code description, Fix profile title for pdex-provenance. Change Pdex Provenance to derive from R4 Provenance. Fix menu bar layout.  FHIR-29594 - Add PDex Server CapabilityStatement, Update FDA National Drug Code ValueSet to match CARIN-BB.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pdex-provenance.xlsx
+++ b/output/StructureDefinition-pdex-provenance.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$39</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="288">
   <si>
     <t>Path</t>
   </si>
@@ -141,7 +141,7 @@
   </si>
   <si>
     <t>History
-EventActivityBasic Provenance</t>
+EventActivity</t>
   </si>
   <si>
     <t>0</t>
@@ -153,10 +153,10 @@
     <t/>
   </si>
   <si>
-    <t>US Core Provenance</t>
-  </si>
-  <si>
-    <t>The US Core Provenance Profile is based upon the Argonaut Data Query requirements.</t>
+    <t>Who, What, When for a set of resources</t>
+  </si>
+  <si>
+    <t>Provenance of a resource is a record that describes entities and processes involved in producing and delivering or otherwise influencing that resource. Provenance provides a critical foundation for assessing authenticity, enabling trust, and allowing reproducibility. Provenance assertions are a form of contextual metadata and can themselves become important records with their own provenance. Provenance statement indicates clinical significance in terms of confidence in authenticity, reliability, and trustworthiness, integrity, and stage in lifecycle (e.g. Document Completion - has the artifact been legally authenticated), all of which may impact security, privacy, and trust policies.</t>
   </si>
   <si>
     <t>Some parties may be duplicated between the target resource and its provenance.  For instance, the prescriber is usually (but not always) the author of the prescription resource. This resource is defined with close consideration for W3C Provenance.</t>
@@ -369,7 +369,7 @@
 </t>
   </si>
   <si>
-    <t>The Resource this Provenance record supports</t>
+    <t>Target Reference(s) (usually version specific)</t>
   </si>
   <si>
     <t>The Reference(s) that were generated or updated by  the activity described in this resource. A provenance can point to more than one target if multiple resources were created/updated by the same activity.</t>
@@ -569,13 +569,6 @@
     <t>An agent can be a person, an organization, software, device, or other entities that may be ascribed responsibility.</t>
   </si>
   <si>
-    <t xml:space="preserve">pattern:type}
-</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>Event.performer</t>
   </si>
   <si>
@@ -717,62 +710,20 @@
     <t>Provenance.agent.onBehalfOf</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization)
-</t>
-  </si>
-  <si>
-    <t>Who the agent is representing</t>
-  </si>
-  <si>
-    <t>The individual, device, or organization for whom the change was made.</t>
-  </si>
-  <si>
-    <t>onBehalfOfIdentity should be used when the agent is not a Resource type.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-provenance-1:onBehalfOf SHALL be present when Provenance.agent.who is a Practitioner or Device {(($this.agent.who.resolve() is Practitioner) or ($this.agent.who.resolve() is Device)) implies exists()}</t>
-  </si>
-  <si>
-    <t>Person, Practitioner, Organization, Device :* .role [classCode = RoleClassMutualRelationship; role.code and * .scopes[Role](classCode=IDENT) and *.plays [Role.Code]</t>
-  </si>
-  <si>
-    <t>ProvenanceAuthor</t>
-  </si>
-  <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://terminology.hl7.org/CodeSystem/provenance-participant-type"/&gt;
-    &lt;code value="author"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>The type of participation that a provenance agent played with respect to the activity.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/provenance-agent-type</t>
-  </si>
-  <si>
-    <t>Who participated</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reference(Practitioner|PractitionerRole|RelatedPerson|Patient|Device|Organization)
 </t>
   </si>
   <si>
-    <t>ProvenanceTransmitter</t>
-  </si>
-  <si>
-    <t>The entity that provided the copy to your system.</t>
-  </si>
-  <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://hl7.org/fhir/us/core/CodeSystem/us-core-provenance-participant-type"/&gt;
-    &lt;code value="transmitter"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
+    <t>Who the agent is representing</t>
+  </si>
+  <si>
+    <t>The individual, device, or organization for whom the change was made.</t>
+  </si>
+  <si>
+    <t>onBehalfOfIdentity should be used when the agent is not a Resource type.</t>
+  </si>
+  <si>
+    <t>Person, Practitioner, Organization, Device :* .role [classCode = RoleClassMutualRelationship; role.code and * .scopes[Role](classCode=IDENT) and *.plays [Role.Code]</t>
   </si>
   <si>
     <t>Provenance.entity</t>
@@ -807,6 +758,9 @@
   <si>
     <t xml:space="preserve">value:url}
 </t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>sourceFormat</t>
@@ -1103,7 +1057,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN55"/>
+  <dimension ref="A1:AN39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1113,7 +1067,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="37.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="23.05078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.5" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
@@ -1135,7 +1089,7 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="81.1875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="65.578125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="74.5390625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
@@ -2302,7 +2256,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>110</v>
       </c>
@@ -2318,7 +2272,7 @@
         <v>43</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>44</v>
@@ -2530,7 +2484,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>128</v>
       </c>
@@ -2546,7 +2500,7 @@
         <v>53</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>44</v>
@@ -3110,7 +3064,7 @@
         <v>43</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>44</v>
@@ -3168,14 +3122,16 @@
         <v>44</v>
       </c>
       <c r="AA18" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="AB18" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB18" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC18" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD18" t="s" s="2">
-        <v>178</v>
+        <v>44</v>
       </c>
       <c r="AE18" t="s" s="2">
         <v>171</v>
@@ -3193,24 +3149,24 @@
         <v>65</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AL18" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AN18" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="AN18" t="s" s="2">
-        <v>183</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3236,10 +3192,10 @@
         <v>55</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3290,7 +3246,7 @@
         <v>44</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>42</v>
@@ -3308,7 +3264,7 @@
         <v>44</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>44</v>
@@ -3322,7 +3278,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3351,7 +3307,7 @@
         <v>100</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M20" t="s" s="2">
         <v>102</v>
@@ -3404,7 +3360,7 @@
         <v>44</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>42</v>
@@ -3422,7 +3378,7 @@
         <v>44</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>44</v>
@@ -3436,11 +3392,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3462,10 +3418,10 @@
         <v>99</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M21" t="s" s="2">
         <v>102</v>
@@ -3520,7 +3476,7 @@
         <v>44</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>42</v>
@@ -3550,9 +3506,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3566,7 +3522,7 @@
         <v>53</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>44</v>
@@ -3578,13 +3534,13 @@
         <v>153</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="M22" t="s" s="2">
         <v>198</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -3610,11 +3566,11 @@
         <v>44</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>44</v>
@@ -3632,7 +3588,7 @@
         <v>44</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>42</v>
@@ -3647,24 +3603,24 @@
         <v>65</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="AK22" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="AL22" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN22" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>206</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3690,13 +3646,13 @@
         <v>153</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="M23" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>210</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -3722,14 +3678,14 @@
         <v>44</v>
       </c>
       <c r="W23" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="X23" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="Y23" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="X23" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="Y23" t="s" s="2">
-        <v>213</v>
-      </c>
       <c r="Z23" t="s" s="2">
         <v>44</v>
       </c>
@@ -3746,7 +3702,7 @@
         <v>44</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>42</v>
@@ -3764,7 +3720,7 @@
         <v>44</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>44</v>
@@ -3773,12 +3729,12 @@
         <v>44</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3801,16 +3757,16 @@
         <v>54</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3860,7 +3816,7 @@
         <v>44</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>53</v>
@@ -3875,24 +3831,24 @@
         <v>65</v>
       </c>
       <c r="AJ24" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AK24" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AL24" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM24" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="AK24" t="s" s="2">
+      <c r="AN24" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" hidden="true">
+      <c r="A25" t="s" s="2">
         <v>222</v>
-      </c>
-      <c r="AL24" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM24" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3906,7 +3862,7 @@
         <v>53</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>44</v>
@@ -3915,16 +3871,16 @@
         <v>44</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="K25" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>228</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3974,7 +3930,7 @@
         <v>44</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>42</v>
@@ -3986,13 +3942,13 @@
         <v>44</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>229</v>
+        <v>65</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>44</v>
@@ -4004,13 +3960,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="B26" t="s" s="2">
-        <v>231</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
         <v>44</v>
       </c>
@@ -4022,7 +3976,7 @@
         <v>43</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>44</v>
@@ -4034,17 +3988,13 @@
         <v>172</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>173</v>
+        <v>229</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>176</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>44</v>
       </c>
@@ -4092,10 +4042,10 @@
         <v>44</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>171</v>
+        <v>228</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>43</v>
@@ -4107,24 +4057,24 @@
         <v>65</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>179</v>
+        <v>44</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>180</v>
+        <v>231</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>181</v>
+        <v>232</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>182</v>
+        <v>44</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>183</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>184</v>
+        <v>234</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4150,10 +4100,10 @@
         <v>55</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4204,7 +4154,7 @@
         <v>44</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>42</v>
@@ -4222,7 +4172,7 @@
         <v>44</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>44</v>
@@ -4236,11 +4186,11 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4262,14 +4212,12 @@
         <v>99</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>100</v>
+        <v>236</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>44</v>
@@ -4306,19 +4254,17 @@
         <v>44</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB28" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="AB28" s="2"/>
       <c r="AC28" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>44</v>
+        <v>239</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>42</v>
@@ -4336,7 +4282,7 @@
         <v>44</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>188</v>
+        <v>44</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>44</v>
@@ -4348,45 +4294,43 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>240</v>
+      </c>
       <c r="C29" t="s" s="2">
-        <v>193</v>
+        <v>44</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I29" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>99</v>
+        <v>241</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>194</v>
+        <v>242</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>44</v>
       </c>
@@ -4434,7 +4378,7 @@
         <v>44</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
@@ -4443,7 +4387,7 @@
         <v>43</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>44</v>
+        <v>244</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>104</v>
@@ -4464,9 +4408,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>197</v>
+        <v>245</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4474,32 +4418,30 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>53</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>153</v>
+        <v>55</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>200</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>44</v>
@@ -4509,7 +4451,7 @@
         <v>44</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>232</v>
+        <v>44</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>44</v>
@@ -4524,13 +4466,13 @@
         <v>44</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>233</v>
+        <v>44</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>234</v>
+        <v>44</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>44</v>
@@ -4548,7 +4490,7 @@
         <v>44</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>42</v>
@@ -4560,27 +4502,27 @@
         <v>44</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>203</v>
+        <v>44</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>205</v>
+        <v>44</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>206</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4591,7 +4533,7 @@
         <v>42</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>44</v>
@@ -4603,17 +4545,15 @@
         <v>44</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>153</v>
+        <v>99</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>208</v>
+        <v>236</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>210</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>44</v>
@@ -4638,31 +4578,31 @@
         <v>44</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>212</v>
+        <v>44</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>213</v>
+        <v>44</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AA31" t="s" s="2">
-        <v>44</v>
+        <v>238</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>44</v>
+        <v>247</v>
       </c>
       <c r="AC31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD31" t="s" s="2">
-        <v>44</v>
+        <v>239</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>42</v>
@@ -4674,13 +4614,13 @@
         <v>44</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>214</v>
+        <v>44</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>44</v>
@@ -4689,12 +4629,12 @@
         <v>44</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>215</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4708,25 +4648,25 @@
         <v>53</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>217</v>
+        <v>67</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4734,7 +4674,7 @@
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
-        <v>44</v>
+        <v>252</v>
       </c>
       <c r="R32" t="s" s="2">
         <v>44</v>
@@ -4776,7 +4716,7 @@
         <v>44</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>216</v>
+        <v>253</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>53</v>
@@ -4788,19 +4728,19 @@
         <v>44</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>221</v>
+        <v>44</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>222</v>
+        <v>96</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>223</v>
+        <v>44</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>44</v>
@@ -4808,7 +4748,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4831,17 +4771,15 @@
         <v>44</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>236</v>
+        <v>153</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>226</v>
+        <v>255</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>228</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>44</v>
@@ -4878,19 +4816,17 @@
         <v>44</v>
       </c>
       <c r="AA33" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="AB33" s="2"/>
       <c r="AC33" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD33" t="s" s="2">
-        <v>44</v>
+        <v>258</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>42</v>
@@ -4908,7 +4844,7 @@
         <v>44</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>230</v>
+        <v>96</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>44</v>
@@ -4920,12 +4856,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>171</v>
+        <v>254</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>44</v>
@@ -4938,7 +4874,7 @@
         <v>53</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>44</v>
@@ -4947,20 +4883,16 @@
         <v>44</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>173</v>
+        <v>261</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>176</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>44</v>
       </c>
@@ -4984,13 +4916,11 @@
         <v>44</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X34" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="X34" s="2"/>
       <c r="Y34" t="s" s="2">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>44</v>
@@ -5008,13 +4938,13 @@
         <v>44</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>171</v>
+        <v>259</v>
       </c>
       <c r="AF34" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG34" t="s" s="2">
         <v>53</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>43</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>44</v>
@@ -5023,56 +4953,60 @@
         <v>65</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>179</v>
+        <v>44</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>180</v>
+        <v>96</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>181</v>
+        <v>44</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>182</v>
+        <v>44</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>183</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>184</v>
+        <v>263</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>44</v>
+        <v>191</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+        <v>193</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>44</v>
       </c>
@@ -5120,25 +5054,25 @@
         <v>44</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>188</v>
+        <v>96</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>44</v>
@@ -5152,18 +5086,18 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>189</v>
+        <v>264</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>44</v>
@@ -5172,20 +5106,18 @@
         <v>44</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>100</v>
+        <v>265</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>44</v>
@@ -5210,13 +5142,13 @@
         <v>44</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>44</v>
+        <v>267</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>44</v>
+        <v>268</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>44</v>
@@ -5234,75 +5166,73 @@
         <v>44</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>191</v>
+        <v>264</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>188</v>
+        <v>269</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>44</v>
+        <v>270</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>44</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>192</v>
+        <v>272</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>193</v>
+        <v>44</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I37" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>194</v>
+        <v>273</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>195</v>
+        <v>274</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>44</v>
       </c>
@@ -5350,39 +5280,39 @@
         <v>44</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>96</v>
+        <v>276</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>44</v>
+        <v>277</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>44</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>197</v>
+        <v>278</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5390,31 +5320,31 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>198</v>
+        <v>279</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>199</v>
+        <v>280</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>200</v>
+        <v>281</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -5425,7 +5355,7 @@
         <v>44</v>
       </c>
       <c r="R38" t="s" s="2">
-        <v>239</v>
+        <v>44</v>
       </c>
       <c r="S38" t="s" s="2">
         <v>44</v>
@@ -5440,13 +5370,13 @@
         <v>44</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>233</v>
+        <v>44</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>234</v>
+        <v>44</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>44</v>
@@ -5464,13 +5394,13 @@
         <v>44</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>197</v>
+        <v>278</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>44</v>
@@ -5479,24 +5409,24 @@
         <v>65</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>203</v>
+        <v>44</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>204</v>
+        <v>282</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>205</v>
+        <v>44</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>206</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5519,17 +5449,15 @@
         <v>44</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>153</v>
+        <v>284</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>208</v>
+        <v>285</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>210</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>44</v>
@@ -5554,13 +5482,13 @@
         <v>44</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>212</v>
+        <v>44</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>213</v>
+        <v>44</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>44</v>
@@ -5578,7 +5506,7 @@
         <v>44</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>42</v>
@@ -5596,7 +5524,7 @@
         <v>44</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>214</v>
+        <v>287</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>44</v>
@@ -5605,1815 +5533,11 @@
         <v>44</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="F40" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G40" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="H40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I40" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="J40" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P40" s="2"/>
-      <c r="Q40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AN40" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" hidden="true">
-      <c r="A41" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F41" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J41" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="K41" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="N41" s="2"/>
-      <c r="O41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P41" s="2"/>
-      <c r="Q41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN41" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" hidden="true">
-      <c r="A42" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J42" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P42" s="2"/>
-      <c r="Q42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE42" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="AF42" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="AM42" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN42" t="s" s="2">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="43" hidden="true">
-      <c r="A43" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F43" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J43" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="K43" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P43" s="2"/>
-      <c r="Q43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE43" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK43" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="AL43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN43" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" hidden="true">
-      <c r="A44" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J44" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="K44" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P44" s="2"/>
-      <c r="Q44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="AB44" s="2"/>
-      <c r="AC44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="AF44" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG44" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI44" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AJ44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM44" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="C45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F45" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G45" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="H45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J45" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="K45" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P45" s="2"/>
-      <c r="Q45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE45" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="AF45" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG45" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH45" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="AI45" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AJ45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK45" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AL45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN45" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" hidden="true">
-      <c r="A46" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F46" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J46" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="K46" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P46" s="2"/>
-      <c r="Q46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE46" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="AF46" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG46" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK46" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="AL46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN46" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" hidden="true">
-      <c r="A47" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J47" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="K47" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P47" s="2"/>
-      <c r="Q47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA47" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="AB47" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="AC47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="AF47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG47" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI47" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AJ47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" hidden="true">
-      <c r="A48" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="F48" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J48" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="K48" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="N48" s="2"/>
-      <c r="O48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P48" s="2"/>
-      <c r="Q48" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="R48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE48" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="AF48" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AG48" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AL48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" hidden="true">
-      <c r="A49" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F49" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J49" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="K49" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P49" s="2"/>
-      <c r="Q49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA49" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="AB49" s="2"/>
-      <c r="AC49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD49" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AE49" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="AF49" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG49" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI49" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK49" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AL49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" hidden="true">
-      <c r="A50" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="B50" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="C50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F50" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J50" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P50" s="2"/>
-      <c r="Q50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W50" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="X50" s="2"/>
-      <c r="Y50" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="Z50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG50" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI50" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AL50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" hidden="true">
-      <c r="A51" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F51" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H51" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="I51" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="J51" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P51" s="2"/>
-      <c r="Q51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="AF51" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG51" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AJ51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" hidden="true">
-      <c r="A52" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="F52" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I52" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="J52" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="K52" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P52" s="2"/>
-      <c r="Q52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W52" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="X52" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="Y52" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AG52" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI52" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN52" t="s" s="2">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="53" hidden="true">
-      <c r="A53" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="F53" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I53" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="J53" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="K53" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="N53" s="2"/>
-      <c r="O53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P53" s="2"/>
-      <c r="Q53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="AF53" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AG53" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="AH53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN53" t="s" s="2">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" hidden="true">
-      <c r="A54" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="N54" s="2"/>
-      <c r="O54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN54" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" hidden="true">
-      <c r="A55" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J55" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P55" s="2"/>
-      <c r="Q55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE55" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="AF55" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI55" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AK55" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN55" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN55">
+  <autoFilter ref="A1:AN39">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7423,7 +5547,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI54">
+  <conditionalFormatting sqref="A2:AI38">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
v1.0.0 -rev(i) update to switch to us-core base for pdex-provenance. Also changed index.md and pdex-provenance.md. Updated ignoreWarnings.txt for FHIR-29796 reflecting CPG vote to accept pdex-device.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-pdex-provenance.xlsx
+++ b/output/StructureDefinition-pdex-provenance.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$55</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="299">
   <si>
     <t>Path</t>
   </si>
@@ -141,7 +141,7 @@
   </si>
   <si>
     <t>History
-EventActivity</t>
+EventActivityBasic Provenance</t>
   </si>
   <si>
     <t>0</t>
@@ -153,10 +153,10 @@
     <t/>
   </si>
   <si>
-    <t>Who, What, When for a set of resources</t>
-  </si>
-  <si>
-    <t>Provenance of a resource is a record that describes entities and processes involved in producing and delivering or otherwise influencing that resource. Provenance provides a critical foundation for assessing authenticity, enabling trust, and allowing reproducibility. Provenance assertions are a form of contextual metadata and can themselves become important records with their own provenance. Provenance statement indicates clinical significance in terms of confidence in authenticity, reliability, and trustworthiness, integrity, and stage in lifecycle (e.g. Document Completion - has the artifact been legally authenticated), all of which may impact security, privacy, and trust policies.</t>
+    <t>US Core Provenance</t>
+  </si>
+  <si>
+    <t>The US Core Provenance Profile is based upon the Argonaut Data Query requirements.</t>
   </si>
   <si>
     <t>Some parties may be duplicated between the target resource and its provenance.  For instance, the prescriber is usually (but not always) the author of the prescription resource. This resource is defined with close consideration for W3C Provenance.</t>
@@ -369,7 +369,7 @@
 </t>
   </si>
   <si>
-    <t>Target Reference(s) (usually version specific)</t>
+    <t>The Resource this Provenance record supports</t>
   </si>
   <si>
     <t>The Reference(s) that were generated or updated by  the activity described in this resource. A provenance can point to more than one target if multiple resources were created/updated by the same activity.</t>
@@ -569,6 +569,13 @@
     <t>An agent can be a person, an organization, software, device, or other entities that may be ascribed responsibility.</t>
   </si>
   <si>
+    <t xml:space="preserve">pattern:type}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
     <t>Event.performer</t>
   </si>
   <si>
@@ -637,10 +644,7 @@
     <t>For example: author, performer, enterer, attester, etc.</t>
   </si>
   <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pdex/ValueSet/ProvenanceAgentType</t>
+    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-provenance-participant-type</t>
   </si>
   <si>
     <t>Event.performer.function</t>
@@ -710,20 +714,62 @@
     <t>Provenance.agent.onBehalfOf</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization)
+</t>
+  </si>
+  <si>
+    <t>Who the agent is representing</t>
+  </si>
+  <si>
+    <t>The individual, device, or organization for whom the change was made.</t>
+  </si>
+  <si>
+    <t>onBehalfOfIdentity should be used when the agent is not a Resource type.</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+provenance-1:onBehalfOf SHALL be present when Provenance.agent.who is a Practitioner or Device {($this.agent.who.resolve().is Practitioner or Device) implies exists()}</t>
+  </si>
+  <si>
+    <t>Person, Practitioner, Organization, Device :* .role [classCode = RoleClassMutualRelationship; role.code and * .scopes[Role](classCode=IDENT) and *.plays [Role.Code]</t>
+  </si>
+  <si>
+    <t>ProvenanceAuthor</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://terminology.hl7.org/CodeSystem/provenance-participant-type"/&gt;
+    &lt;code value="author"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
+    <t>The type of participation that a provenance agent played with respect to the activity.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/provenance-agent-type</t>
+  </si>
+  <si>
+    <t>Who participated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reference(Practitioner|PractitionerRole|RelatedPerson|Patient|Device|Organization)
 </t>
   </si>
   <si>
-    <t>Who the agent is representing</t>
-  </si>
-  <si>
-    <t>The individual, device, or organization for whom the change was made.</t>
-  </si>
-  <si>
-    <t>onBehalfOfIdentity should be used when the agent is not a Resource type.</t>
-  </si>
-  <si>
-    <t>Person, Practitioner, Organization, Device :* .role [classCode = RoleClassMutualRelationship; role.code and * .scopes[Role](classCode=IDENT) and *.plays [Role.Code]</t>
+    <t>ProvenanceTransmitter</t>
+  </si>
+  <si>
+    <t>The entity that provided the copy to your system.</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://hl7.org/fhir/us/core/CodeSystem/us-core-provenance-participant-type"/&gt;
+    &lt;code value="transmitter"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>Provenance.entity</t>
@@ -760,9 +806,6 @@
 </t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>sourceFormat</t>
   </si>
   <si>
@@ -830,6 +873,9 @@
   </si>
   <si>
     <t>Value of extension</t>
+  </si>
+  <si>
+    <t>required</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/davinci-pdex/ValueSet/ProvenancePayerSourceFormat</t>
@@ -1057,7 +1103,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN39"/>
+  <dimension ref="A1:AN55"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1067,7 +1113,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="37.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.5" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="23.05078125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
@@ -1089,7 +1135,7 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="65.578125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="81.1875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="74.5390625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
@@ -2256,7 +2302,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
         <v>110</v>
       </c>
@@ -2272,7 +2318,7 @@
         <v>43</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>44</v>
@@ -2484,7 +2530,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>128</v>
       </c>
@@ -2500,7 +2546,7 @@
         <v>53</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>44</v>
@@ -3064,7 +3110,7 @@
         <v>43</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>44</v>
@@ -3122,16 +3168,14 @@
         <v>44</v>
       </c>
       <c r="AA18" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB18" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="AB18" s="2"/>
       <c r="AC18" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD18" t="s" s="2">
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="AE18" t="s" s="2">
         <v>171</v>
@@ -3149,24 +3193,24 @@
         <v>65</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3192,10 +3236,10 @@
         <v>55</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3246,7 +3290,7 @@
         <v>44</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>42</v>
@@ -3264,7 +3308,7 @@
         <v>44</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>44</v>
@@ -3278,7 +3322,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3307,7 +3351,7 @@
         <v>100</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="M20" t="s" s="2">
         <v>102</v>
@@ -3360,7 +3404,7 @@
         <v>44</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>42</v>
@@ -3378,7 +3422,7 @@
         <v>44</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>44</v>
@@ -3392,11 +3436,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3418,10 +3462,10 @@
         <v>99</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M21" t="s" s="2">
         <v>102</v>
@@ -3476,7 +3520,7 @@
         <v>44</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>42</v>
@@ -3506,9 +3550,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3516,13 +3560,13 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>53</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>44</v>
@@ -3534,13 +3578,13 @@
         <v>153</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -3566,11 +3610,11 @@
         <v>44</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>44</v>
@@ -3588,7 +3632,7 @@
         <v>44</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>42</v>
@@ -3603,24 +3647,24 @@
         <v>65</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3646,13 +3690,13 @@
         <v>153</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -3678,13 +3722,13 @@
         <v>44</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>44</v>
@@ -3702,7 +3746,7 @@
         <v>44</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>42</v>
@@ -3720,7 +3764,7 @@
         <v>44</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>44</v>
@@ -3729,12 +3773,12 @@
         <v>44</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3757,16 +3801,16 @@
         <v>54</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3816,7 +3860,7 @@
         <v>44</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>53</v>
@@ -3831,24 +3875,24 @@
         <v>65</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3862,7 +3906,7 @@
         <v>53</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>44</v>
@@ -3871,16 +3915,16 @@
         <v>44</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3930,7 +3974,7 @@
         <v>44</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>42</v>
@@ -3942,13 +3986,13 @@
         <v>44</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>65</v>
+        <v>228</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>44</v>
@@ -3960,11 +4004,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>230</v>
+      </c>
       <c r="C26" t="s" s="2">
         <v>44</v>
       </c>
@@ -3976,7 +4022,7 @@
         <v>43</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>44</v>
@@ -3988,13 +4034,17 @@
         <v>172</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>229</v>
+        <v>173</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+        <v>174</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="N26" t="s" s="2">
+        <v>176</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>44</v>
       </c>
@@ -4042,10 +4092,10 @@
         <v>44</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>228</v>
+        <v>171</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>43</v>
@@ -4057,24 +4107,24 @@
         <v>65</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>231</v>
+        <v>180</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>232</v>
+        <v>181</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>44</v>
+        <v>182</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>233</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4100,10 +4150,10 @@
         <v>55</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4154,7 +4204,7 @@
         <v>44</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>42</v>
@@ -4172,7 +4222,7 @@
         <v>44</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>44</v>
@@ -4186,11 +4236,11 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>235</v>
+        <v>189</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4212,12 +4262,14 @@
         <v>99</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>236</v>
+        <v>100</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="M28" s="2"/>
+        <v>190</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>44</v>
@@ -4254,17 +4306,19 @@
         <v>44</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="AB28" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC28" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>239</v>
+        <v>44</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>42</v>
@@ -4282,7 +4336,7 @@
         <v>44</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>44</v>
@@ -4294,43 +4348,45 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="B29" t="s" s="2">
-        <v>240</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>44</v>
+        <v>193</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G29" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H29" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="H29" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="I29" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>241</v>
+        <v>99</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>242</v>
+        <v>194</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>44</v>
       </c>
@@ -4378,7 +4434,7 @@
         <v>44</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
@@ -4387,7 +4443,7 @@
         <v>43</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>244</v>
+        <v>44</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>104</v>
@@ -4408,9 +4464,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4418,30 +4474,32 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>53</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="M30" s="2"/>
+        <v>199</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>200</v>
+      </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>44</v>
@@ -4451,7 +4509,7 @@
         <v>44</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>44</v>
@@ -4466,13 +4524,13 @@
         <v>44</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>44</v>
+        <v>233</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>44</v>
@@ -4490,7 +4548,7 @@
         <v>44</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>42</v>
@@ -4502,27 +4560,27 @@
         <v>44</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>44</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4533,7 +4591,7 @@
         <v>42</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>44</v>
@@ -4545,15 +4603,17 @@
         <v>44</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="M31" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>209</v>
+      </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>44</v>
@@ -4578,31 +4638,31 @@
         <v>44</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>44</v>
+        <v>212</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AA31" t="s" s="2">
-        <v>238</v>
+        <v>44</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>247</v>
+        <v>44</v>
       </c>
       <c r="AC31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD31" t="s" s="2">
-        <v>239</v>
+        <v>44</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>42</v>
@@ -4614,13 +4674,13 @@
         <v>44</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>44</v>
+        <v>213</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>44</v>
@@ -4629,12 +4689,12 @@
         <v>44</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>44</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
-        <v>248</v>
+        <v>215</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4648,25 +4708,25 @@
         <v>53</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>67</v>
+        <v>216</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>251</v>
+        <v>219</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4674,7 +4734,7 @@
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
-        <v>252</v>
+        <v>44</v>
       </c>
       <c r="R32" t="s" s="2">
         <v>44</v>
@@ -4716,7 +4776,7 @@
         <v>44</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>53</v>
@@ -4728,19 +4788,19 @@
         <v>44</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>44</v>
+        <v>220</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>96</v>
+        <v>221</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>44</v>
+        <v>222</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>44</v>
@@ -4748,7 +4808,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4771,15 +4831,17 @@
         <v>44</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>153</v>
+        <v>235</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M33" s="2"/>
+        <v>226</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>227</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>44</v>
@@ -4816,17 +4878,19 @@
         <v>44</v>
       </c>
       <c r="AA33" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="AB33" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB33" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC33" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD33" t="s" s="2">
-        <v>258</v>
+        <v>44</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>42</v>
@@ -4844,7 +4908,7 @@
         <v>44</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>96</v>
+        <v>229</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>44</v>
@@ -4856,12 +4920,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" hidden="true">
+    <row r="34">
       <c r="A34" t="s" s="2">
-        <v>254</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>44</v>
@@ -4874,7 +4938,7 @@
         <v>53</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>44</v>
@@ -4883,16 +4947,20 @@
         <v>44</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>261</v>
+        <v>173</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+        <v>237</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>176</v>
+      </c>
       <c r="O34" t="s" s="2">
         <v>44</v>
       </c>
@@ -4916,11 +4984,13 @@
         <v>44</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="X34" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="X34" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="Y34" t="s" s="2">
-        <v>262</v>
+        <v>44</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>44</v>
@@ -4938,13 +5008,13 @@
         <v>44</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>259</v>
+        <v>171</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>44</v>
@@ -4953,60 +5023,56 @@
         <v>65</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>96</v>
+        <v>180</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>44</v>
+        <v>182</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>44</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>263</v>
+        <v>184</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>191</v>
+        <v>44</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>44</v>
       </c>
@@ -5054,25 +5120,25 @@
         <v>44</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>44</v>
@@ -5086,18 +5152,18 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>264</v>
+        <v>189</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>44</v>
@@ -5106,18 +5172,20 @@
         <v>44</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>265</v>
+        <v>100</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="M36" s="2"/>
+        <v>190</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>44</v>
@@ -5142,13 +5210,13 @@
         <v>44</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>199</v>
+        <v>44</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>267</v>
+        <v>44</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>268</v>
+        <v>44</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>44</v>
@@ -5166,73 +5234,75 @@
         <v>44</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>264</v>
+        <v>191</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>269</v>
+        <v>188</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>270</v>
+        <v>44</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>271</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>272</v>
+        <v>192</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>44</v>
+        <v>193</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="I37" t="s" s="2">
         <v>54</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>273</v>
+        <v>194</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>274</v>
+        <v>195</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="N37" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="O37" t="s" s="2">
         <v>44</v>
       </c>
@@ -5280,39 +5350,39 @@
         <v>44</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>272</v>
+        <v>196</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>276</v>
+        <v>96</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>277</v>
+        <v>44</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>118</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
-        <v>278</v>
+        <v>197</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5320,31 +5390,31 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>279</v>
+        <v>198</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>280</v>
+        <v>199</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>281</v>
+        <v>200</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -5355,7 +5425,7 @@
         <v>44</v>
       </c>
       <c r="R38" t="s" s="2">
-        <v>44</v>
+        <v>238</v>
       </c>
       <c r="S38" t="s" s="2">
         <v>44</v>
@@ -5370,13 +5440,13 @@
         <v>44</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>44</v>
+        <v>233</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>44</v>
@@ -5394,13 +5464,13 @@
         <v>44</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>278</v>
+        <v>197</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>44</v>
@@ -5409,24 +5479,24 @@
         <v>65</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>282</v>
+        <v>203</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>44</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>283</v>
+        <v>206</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5449,15 +5519,17 @@
         <v>44</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>285</v>
+        <v>207</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M39" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>209</v>
+      </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>44</v>
@@ -5482,13 +5554,13 @@
         <v>44</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>44</v>
+        <v>212</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>44</v>
@@ -5506,7 +5578,7 @@
         <v>44</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>283</v>
+        <v>206</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>42</v>
@@ -5524,20 +5596,1824 @@
         <v>44</v>
       </c>
       <c r="AK39" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="AL39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN39" t="s" s="2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G40" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="H40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I40" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J40" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="N40" s="2"/>
+      <c r="O40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P40" s="2"/>
+      <c r="Q40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AL40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM40" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AN40" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" hidden="true">
+      <c r="A41" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F41" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J41" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="N41" s="2"/>
+      <c r="O41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P41" s="2"/>
+      <c r="Q41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN41" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J42" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P42" s="2"/>
+      <c r="Q42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE42" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="AL42" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="AM42" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN42" t="s" s="2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" hidden="true">
+      <c r="A43" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F43" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J43" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P43" s="2"/>
+      <c r="Q43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AL43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM43" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN43" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" hidden="true">
+      <c r="A44" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J44" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P44" s="2"/>
+      <c r="Q44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="AB44" s="2"/>
+      <c r="AC44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM44" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN44" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F45" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P45" s="2"/>
+      <c r="Q45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE45" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN45" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" hidden="true">
+      <c r="A46" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F46" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J46" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P46" s="2"/>
+      <c r="Q46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN46" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" hidden="true">
+      <c r="A47" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P47" s="2"/>
+      <c r="Q47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" hidden="true">
+      <c r="A48" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F48" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="N48" s="2"/>
+      <c r="O48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P48" s="2"/>
+      <c r="Q48" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="R48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" hidden="true">
+      <c r="A49" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F49" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J49" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P49" s="2"/>
+      <c r="Q49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AB49" s="2"/>
+      <c r="AC49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" hidden="true">
+      <c r="A50" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F50" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P50" s="2"/>
+      <c r="Q50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="X50" s="2"/>
+      <c r="Y50" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN50" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" hidden="true">
+      <c r="A51" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F51" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H51" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J51" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE51" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="N53" s="2"/>
+      <c r="O53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK53" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="AL39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN39" t="s" s="2">
+      <c r="AL53" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="N54" s="2"/>
+      <c r="O54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN55" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN39">
+  <autoFilter ref="A1:AN55">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5547,7 +7423,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI38">
+  <conditionalFormatting sqref="A2:AI54">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>